<commit_message>
Comparativa de modelos físicos. Eliminados archivos viejos del repositorio.
</commit_message>
<xml_diff>
--- a/Modelo físico/ComparacionModelosFisicosDraganflyerV_Referencias.xlsx
+++ b/Modelo físico/ComparacionModelosFisicosDraganflyerV_Referencias.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="62">
   <si>
     <t>Criterio</t>
   </si>
@@ -66,9 +66,6 @@
     <t>¿Cómo se manejan las rotaciones?</t>
   </si>
   <si>
-    <t>Direction Cosine Matrix (DCM).</t>
-  </si>
-  <si>
     <t>Arda Ozgur</t>
   </si>
   <si>
@@ -144,9 +141,6 @@
     <t>Modela las salidas de los actuadores como aceleraciones (En pitch, roll, yaw y elevación vertical) en función de las fuerzas que producen, la longitud de los ejes de horizontales, y la masa del  cuadricóptero.</t>
   </si>
   <si>
-    <t>Condición de vuelo, ángulos y velocidades angulares, posición y velocidades lineales iguales a 0.</t>
-  </si>
-  <si>
     <t>Muy bueno!</t>
   </si>
   <si>
@@ -187,6 +181,27 @@
   </si>
   <si>
     <t>Venditelli</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Condición de vuelo, y ángulos y velocidades angulares, posición y velocidades lineales iniciales iguales a 0.</t>
+  </si>
+  <si>
+    <t>Excelente, pero muy complejo.</t>
+  </si>
+  <si>
+    <t>Muy bueno, pero simple.</t>
+  </si>
+  <si>
+    <t>¿Por qué éste?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modelo lineal de la relación voltaje-torque de los motores, transformación de velocidades ángulares respecto a la tierra y ángulos de Euler, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Transformación de velocidades ángulares respecto a la tierra y ángulos de Euler, efecto giroscópico, </t>
   </si>
 </sst>
 </file>
@@ -210,12 +225,48 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -230,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -239,13 +290,35 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A4:O27"/>
+  <dimension ref="A4:O28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D20" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -563,21 +636,21 @@
       <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="4"/>
-      <c r="O4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="4"/>
     </row>
     <row r="5" spans="1:15">
       <c r="B5" s="5"/>
@@ -585,25 +658,25 @@
         <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -613,31 +686,31 @@
     </row>
     <row r="6" spans="1:15">
       <c r="A6" s="2"/>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="2" t="s">
+      <c r="J6" s="8" t="s">
         <v>10</v>
       </c>
       <c r="K6" s="2"/>
@@ -648,32 +721,32 @@
     </row>
     <row r="7" spans="1:15" ht="60">
       <c r="A7" s="2"/>
-      <c r="B7" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>38</v>
+      <c r="B7" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="G7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>37</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
@@ -693,16 +766,16 @@
         <v>11</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>11</v>
@@ -728,16 +801,16 @@
         <v>11</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>11</v>
@@ -760,19 +833,19 @@
         <v>13</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>11</v>
@@ -789,31 +862,31 @@
     <row r="11" spans="1:15">
       <c r="A11" s="2"/>
       <c r="B11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>28</v>
-      </c>
       <c r="E11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>22</v>
+        <v>27</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J11" s="2" t="s">
-        <v>11</v>
+      <c r="J11" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
@@ -823,31 +896,31 @@
     </row>
     <row r="12" spans="1:15" ht="60">
       <c r="A12" s="2"/>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="H12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="8" t="s">
         <v>12</v>
       </c>
       <c r="K12" s="2"/>
@@ -865,25 +938,25 @@
         <v>11</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
@@ -893,29 +966,31 @@
     </row>
     <row r="14" spans="1:15" ht="45">
       <c r="A14" s="2"/>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2" t="s">
+      <c r="F14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="G14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="H14" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="I14" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" s="8" t="s">
         <v>14</v>
       </c>
       <c r="K14" s="2"/>
@@ -926,30 +1001,32 @@
     </row>
     <row r="15" spans="1:15" ht="30">
       <c r="A15" s="2"/>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>19</v>
+      <c r="C15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="8" t="s">
+        <v>18</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
@@ -959,30 +1036,32 @@
     </row>
     <row r="16" spans="1:15" ht="75">
       <c r="A16" s="2"/>
-      <c r="B16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>42</v>
+      <c r="B16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G16" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>56</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
@@ -992,30 +1071,30 @@
     </row>
     <row r="17" spans="1:15" ht="45">
       <c r="A17" s="2"/>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>23</v>
+      <c r="D17" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>22</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
@@ -1025,29 +1104,29 @@
     </row>
     <row r="18" spans="1:15">
       <c r="A18" s="2"/>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J18" s="2" t="s">
+      <c r="F18" s="8"/>
+      <c r="G18" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="J18" s="8" t="s">
         <v>11</v>
       </c>
       <c r="K18" s="2"/>
@@ -1059,20 +1138,20 @@
     <row r="19" spans="1:15" ht="75">
       <c r="A19" s="2"/>
       <c r="B19" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>31</v>
-      </c>
       <c r="F19" s="2"/>
-      <c r="G19" s="2" t="s">
-        <v>30</v>
+      <c r="G19" s="12" t="s">
+        <v>29</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>11</v>
@@ -1092,26 +1171,24 @@
     <row r="20" spans="1:15" ht="120">
       <c r="A20" s="2"/>
       <c r="B20" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-      <c r="E20" s="2" t="s">
-        <v>41</v>
+      <c r="E20" s="10" t="s">
+        <v>40</v>
       </c>
       <c r="F20" s="2"/>
-      <c r="G20" s="2" t="s">
-        <v>41</v>
+      <c r="G20" s="11" t="s">
+        <v>40</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="J20" s="2" t="s">
-        <v>11</v>
-      </c>
+      <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
       <c r="M20" s="2"/>
@@ -1173,19 +1250,19 @@
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D24" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="G24" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -1216,26 +1293,32 @@
     <row r="26" spans="1:15" ht="45">
       <c r="A26" s="2"/>
       <c r="B26" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C26" s="2"/>
+        <v>48</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>58</v>
+      </c>
       <c r="D26" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I26" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J26" s="2"/>
+      <c r="J26" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
       <c r="M26" s="2"/>
@@ -1244,28 +1327,42 @@
     </row>
     <row r="27" spans="1:15">
       <c r="B27" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>40</v>
+        <v>55</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G27" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G27" s="13" t="s">
+        <v>39</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J27" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
+      </c>
+      <c r="J27" s="13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="75">
+      <c r="B28" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="J28" s="14" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Documento - Sistemas de control - Modelo dinámico.
</commit_message>
<xml_diff>
--- a/Modelo físico/ComparacionModelosFisicosDraganflyerV_Referencias.xlsx
+++ b/Modelo físico/ComparacionModelosFisicosDraganflyerV_Referencias.xlsx
@@ -27,9 +27,6 @@
     <t>Efecto de los movimientos de traslación sobre el cuerpo</t>
   </si>
   <si>
-    <t>Efecto piso</t>
-  </si>
-  <si>
     <t>Flapping de las hélices</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>Arda Ozgur</t>
   </si>
   <si>
-    <t>Asunciones especiales</t>
-  </si>
-  <si>
     <t>Matriz de rotación 3D RzRyRx.</t>
   </si>
   <si>
@@ -187,6 +181,12 @@
   </si>
   <si>
     <t>Venditelli</t>
+  </si>
+  <si>
+    <t>Efecto suelo</t>
+  </si>
+  <si>
+    <t>Condiciones iniciales</t>
   </si>
 </sst>
 </file>
@@ -218,7 +218,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -226,11 +226,136 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -239,13 +364,37 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,10 +689,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A4:O27"/>
+  <dimension ref="A3:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D20" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -559,51 +708,52 @@
     <col min="10" max="10" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:15">
+    <row r="3" spans="1:15" ht="15.75" thickBot="1"/>
+    <row r="4" spans="1:15" ht="15.75" thickBot="1">
       <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="8"/>
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
-      <c r="O4" s="6"/>
-    </row>
-    <row r="5" spans="1:15">
-      <c r="B5" s="5"/>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>56</v>
+      <c r="O4" s="4"/>
+    </row>
+    <row r="5" spans="1:15" ht="15.75" thickBot="1">
+      <c r="B5" s="9"/>
+      <c r="C5" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="I5" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>54</v>
       </c>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -611,34 +761,34 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
     </row>
-    <row r="6" spans="1:15">
+    <row r="6" spans="1:15" ht="15.75" thickBot="1">
       <c r="A6" s="2"/>
-      <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>10</v>
+      <c r="B6" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>9</v>
       </c>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -646,34 +796,34 @@
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
     </row>
-    <row r="7" spans="1:15" ht="60">
+    <row r="7" spans="1:15" ht="60.75" thickBot="1">
       <c r="A7" s="2"/>
-      <c r="B7" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>38</v>
+      <c r="B7" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>36</v>
       </c>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
@@ -681,34 +831,34 @@
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
     </row>
-    <row r="8" spans="1:15">
+    <row r="8" spans="1:15" ht="15.75" thickBot="1">
       <c r="A8" s="2"/>
-      <c r="B8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>11</v>
+      <c r="B8" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>10</v>
       </c>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -716,34 +866,34 @@
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
     </row>
-    <row r="9" spans="1:15">
+    <row r="9" spans="1:15" ht="15.75" thickBot="1">
       <c r="A9" s="2"/>
-      <c r="B9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>11</v>
+      <c r="B9" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>10</v>
       </c>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -751,34 +901,34 @@
       <c r="N9" s="2"/>
       <c r="O9" s="2"/>
     </row>
-    <row r="10" spans="1:15" ht="30">
+    <row r="10" spans="1:15" ht="30.75" thickBot="1">
       <c r="A10" s="2"/>
-      <c r="B10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>11</v>
+      <c r="B10" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="16" t="s">
+        <v>10</v>
       </c>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -786,34 +936,34 @@
       <c r="N10" s="2"/>
       <c r="O10" s="2"/>
     </row>
-    <row r="11" spans="1:15">
+    <row r="11" spans="1:15" ht="15.75" thickBot="1">
       <c r="A11" s="2"/>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>11</v>
+      <c r="D11" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>10</v>
       </c>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
@@ -821,34 +971,34 @@
       <c r="N11" s="2"/>
       <c r="O11" s="2"/>
     </row>
-    <row r="12" spans="1:15" ht="60">
+    <row r="12" spans="1:15" ht="60.75" thickBot="1">
       <c r="A12" s="2"/>
-      <c r="B12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>12</v>
+      <c r="B12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="16" t="s">
+        <v>11</v>
       </c>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
@@ -856,34 +1006,34 @@
       <c r="N12" s="2"/>
       <c r="O12" s="2"/>
     </row>
-    <row r="13" spans="1:15" ht="45">
+    <row r="13" spans="1:15" ht="45.75" thickBot="1">
       <c r="A13" s="2"/>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>22</v>
+      <c r="C13" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J13" s="16" t="s">
+        <v>20</v>
       </c>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
@@ -891,32 +1041,32 @@
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
     </row>
-    <row r="14" spans="1:15" ht="45">
+    <row r="14" spans="1:15" ht="45.75" thickBot="1">
       <c r="A14" s="2"/>
-      <c r="B14" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>14</v>
+      <c r="B14" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="14"/>
+      <c r="G14" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="H14" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="I14" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>13</v>
       </c>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -924,32 +1074,32 @@
       <c r="N14" s="2"/>
       <c r="O14" s="2"/>
     </row>
-    <row r="15" spans="1:15" ht="30">
+    <row r="15" spans="1:15" ht="30.75" thickBot="1">
       <c r="A15" s="2"/>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>19</v>
+      <c r="D15" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F15" s="14"/>
+      <c r="G15" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="16" t="s">
+        <v>17</v>
       </c>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
@@ -957,32 +1107,32 @@
       <c r="N15" s="2"/>
       <c r="O15" s="2"/>
     </row>
-    <row r="16" spans="1:15" ht="75">
+    <row r="16" spans="1:15" ht="75.75" thickBot="1">
       <c r="A16" s="2"/>
-      <c r="B16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>42</v>
+      <c r="B16" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="14"/>
+      <c r="G16" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="I16" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="J16" s="16" t="s">
+        <v>40</v>
       </c>
       <c r="K16" s="2"/>
       <c r="L16" s="2"/>
@@ -990,32 +1140,32 @@
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
     </row>
-    <row r="17" spans="1:15" ht="45">
+    <row r="17" spans="1:15" ht="45.75" thickBot="1">
       <c r="A17" s="2"/>
-      <c r="B17" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="2" t="s">
+      <c r="B17" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>23</v>
+      <c r="E17" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="14"/>
+      <c r="G17" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H17" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="I17" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J17" s="16" t="s">
+        <v>21</v>
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
@@ -1023,32 +1173,32 @@
       <c r="N17" s="2"/>
       <c r="O17" s="2"/>
     </row>
-    <row r="18" spans="1:15">
+    <row r="18" spans="1:15" ht="15.75" thickBot="1">
       <c r="A18" s="2"/>
-      <c r="B18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="F18" s="2"/>
-      <c r="G18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>11</v>
+      <c r="B18" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" s="14"/>
+      <c r="G18" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J18" s="16" t="s">
+        <v>10</v>
       </c>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
@@ -1056,32 +1206,32 @@
       <c r="N18" s="2"/>
       <c r="O18" s="2"/>
     </row>
-    <row r="19" spans="1:15" ht="75">
+    <row r="19" spans="1:15" ht="75.75" thickBot="1">
       <c r="A19" s="2"/>
-      <c r="B19" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>11</v>
+      <c r="B19" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="14"/>
+      <c r="G19" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="I19" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" s="16" t="s">
+        <v>10</v>
       </c>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
@@ -1089,28 +1239,28 @@
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
     </row>
-    <row r="20" spans="1:15" ht="120">
+    <row r="20" spans="1:15" ht="120.75" thickBot="1">
       <c r="A20" s="2"/>
-      <c r="B20" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="H20" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>11</v>
+      <c r="B20" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="12"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="14"/>
+      <c r="G20" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="I20" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="J20" s="16" t="s">
+        <v>10</v>
       </c>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
@@ -1173,19 +1323,19 @@
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E24" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="G24" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
@@ -1216,24 +1366,24 @@
     <row r="26" spans="1:15" ht="45">
       <c r="A26" s="2"/>
       <c r="B26" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
@@ -1244,34 +1394,34 @@
     </row>
     <row r="27" spans="1:15">
       <c r="B27" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:N4"/>
+    <mergeCell ref="C4:J4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Simulación de los sistemas de control. Documento - Desarrollo: Sistemas de control.
</commit_message>
<xml_diff>
--- a/Modelo físico/ComparacionModelosFisicosDraganflyerV_Referencias.xlsx
+++ b/Modelo físico/ComparacionModelosFisicosDraganflyerV_Referencias.xlsx
@@ -186,7 +186,7 @@
     <t>Efecto suelo</t>
   </si>
   <si>
-    <t>Condiciones iniciales</t>
+    <t>Condiciones iniciales del modelo linealizado</t>
   </si>
 </sst>
 </file>
@@ -691,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A3:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>